<commit_message>
Creación de las posiciones angulares para las 10 iteraciones
</commit_message>
<xml_diff>
--- a/pruebas/DataE1.xlsx
+++ b/pruebas/DataE1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8d97dfd61da619a5/UNAL FORE/SEMESTRE VIII/SERVOMECANISMOS/PROYECTO ACADEMICO/Servomecanismo2R/pruebas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="11_B831B7D75D1BD74478B9349EB34221F6E007CA8D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3389AB48-25B0-4B81-9317-7BF9BCE5A3AA}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="11_B831B7D75D1BD74478B9349EB34221F6E007CA8D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC0ACE02-A45B-4970-96C3-75B01993E9F7}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3795,7 +3795,7 @@
   <dimension ref="A1:R5002"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1088" workbookViewId="0">
-      <selection activeCell="R1112" sqref="R1112"/>
+      <selection activeCell="R1110" sqref="R1110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -20193,7 +20193,7 @@
         <v>10</v>
       </c>
       <c r="R1109">
-        <v>255</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1110" spans="1:18">
@@ -20309,7 +20309,7 @@
       </c>
       <c r="R1112">
         <f>R1107/R1109</f>
-        <v>6.3137254901960782E-4</v>
+        <v>0.161</v>
       </c>
     </row>
     <row r="1113" spans="1:18">

</xml_diff>